<commit_message>
carga: ingreso2, personal, personalxingreso
</commit_message>
<xml_diff>
--- a/Excel/Carga DB Postgres/PersonalXIngreso - cargado.xlsx
+++ b/Excel/Carga DB Postgres/PersonalXIngreso - cargado.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\playa\asd\sugpaDoc\Excel\Carga DB Postgres\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="330" windowWidth="18675" windowHeight="7710" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="336" windowWidth="18672" windowHeight="7716" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="124519" calcMode="manual"/>
 </workbook>
 </file>
 
@@ -32,8 +27,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,7 +63,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -165,7 +190,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -197,10 +222,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -232,7 +256,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -408,19 +431,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -428,7 +451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>20324717928</v>
       </c>
@@ -436,11 +459,11 @@
         <v>1</v>
       </c>
       <c r="D2" t="str">
-        <f>RIGHT(A2,9)</f>
+        <f t="shared" ref="D2:D33" si="0">RIGHT(A2,9)</f>
         <v>324717928</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>27289070406</v>
       </c>
@@ -448,11 +471,11 @@
         <v>2</v>
       </c>
       <c r="D3" t="str">
-        <f>RIGHT(A3,9)</f>
+        <f t="shared" si="0"/>
         <v>289070406</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>27325850820</v>
       </c>
@@ -460,11 +483,11 @@
         <v>3</v>
       </c>
       <c r="D4" t="str">
-        <f>RIGHT(A4,9)</f>
+        <f t="shared" si="0"/>
         <v>325850820</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>20288183784</v>
       </c>
@@ -472,11 +495,11 @@
         <v>4</v>
       </c>
       <c r="D5" t="str">
-        <f>RIGHT(A5,9)</f>
+        <f t="shared" si="0"/>
         <v>288183784</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>23303681329</v>
       </c>
@@ -484,11 +507,11 @@
         <v>5</v>
       </c>
       <c r="D6" t="str">
-        <f>RIGHT(A6,9)</f>
+        <f t="shared" si="0"/>
         <v>303681329</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>23328919249</v>
       </c>
@@ -496,11 +519,11 @@
         <v>6</v>
       </c>
       <c r="D7" t="str">
-        <f>RIGHT(A7,9)</f>
+        <f t="shared" si="0"/>
         <v>328919249</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>27272593103</v>
       </c>
@@ -508,11 +531,11 @@
         <v>7</v>
       </c>
       <c r="D8" t="str">
-        <f>RIGHT(A8,9)</f>
+        <f t="shared" si="0"/>
         <v>272593103</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>27381688599</v>
       </c>
@@ -520,11 +543,11 @@
         <v>8</v>
       </c>
       <c r="D9" t="str">
-        <f>RIGHT(A9,9)</f>
+        <f t="shared" si="0"/>
         <v>381688599</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>23222764114</v>
       </c>
@@ -532,11 +555,11 @@
         <v>9</v>
       </c>
       <c r="D10" t="str">
-        <f>RIGHT(A10,9)</f>
+        <f t="shared" si="0"/>
         <v>222764114</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>27345916453</v>
       </c>
@@ -544,11 +567,11 @@
         <v>10</v>
       </c>
       <c r="D11" t="str">
-        <f>RIGHT(A11,9)</f>
+        <f t="shared" si="0"/>
         <v>345916453</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>27376091029</v>
       </c>
@@ -556,11 +579,11 @@
         <v>11</v>
       </c>
       <c r="D12" t="str">
-        <f>RIGHT(A12,9)</f>
+        <f t="shared" si="0"/>
         <v>376091029</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>23309349369</v>
       </c>
@@ -568,11 +591,11 @@
         <v>12</v>
       </c>
       <c r="D13" t="str">
-        <f>RIGHT(A13,9)</f>
+        <f t="shared" si="0"/>
         <v>309349369</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>20378054002</v>
       </c>
@@ -580,11 +603,11 @@
         <v>13</v>
       </c>
       <c r="D14" t="str">
-        <f>RIGHT(A14,9)</f>
+        <f t="shared" si="0"/>
         <v>378054002</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>27330368921</v>
       </c>
@@ -592,11 +615,11 @@
         <v>14</v>
       </c>
       <c r="D15" t="str">
-        <f>RIGHT(A15,9)</f>
+        <f t="shared" si="0"/>
         <v>330368921</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>27363593475</v>
       </c>
@@ -604,11 +627,11 @@
         <v>15</v>
       </c>
       <c r="D16" t="str">
-        <f>RIGHT(A16,9)</f>
+        <f t="shared" si="0"/>
         <v>363593475</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>27366906369</v>
       </c>
@@ -616,11 +639,11 @@
         <v>16</v>
       </c>
       <c r="D17" t="str">
-        <f>RIGHT(A17,9)</f>
+        <f t="shared" si="0"/>
         <v>366906369</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>20275355535</v>
       </c>
@@ -628,11 +651,11 @@
         <v>17</v>
       </c>
       <c r="D18" t="str">
-        <f>RIGHT(A18,9)</f>
+        <f t="shared" si="0"/>
         <v>275355535</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>27366027926</v>
       </c>
@@ -640,11 +663,11 @@
         <v>18</v>
       </c>
       <c r="D19" t="str">
-        <f>RIGHT(A19,9)</f>
+        <f t="shared" si="0"/>
         <v>366027926</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>27315410970</v>
       </c>
@@ -652,11 +675,11 @@
         <v>19</v>
       </c>
       <c r="D20" t="str">
-        <f>RIGHT(A20,9)</f>
+        <f t="shared" si="0"/>
         <v>315410970</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>20309145802</v>
       </c>
@@ -664,11 +687,11 @@
         <v>20</v>
       </c>
       <c r="D21" t="str">
-        <f>RIGHT(A21,9)</f>
+        <f t="shared" si="0"/>
         <v>309145802</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>27365973720</v>
       </c>
@@ -676,11 +699,11 @@
         <v>21</v>
       </c>
       <c r="D22" t="str">
-        <f>RIGHT(A22,9)</f>
+        <f t="shared" si="0"/>
         <v>365973720</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>20259702349</v>
       </c>
@@ -688,11 +711,11 @@
         <v>22</v>
       </c>
       <c r="D23" t="str">
-        <f>RIGHT(A23,9)</f>
+        <f t="shared" si="0"/>
         <v>259702349</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>27362489100</v>
       </c>
@@ -700,11 +723,11 @@
         <v>23</v>
       </c>
       <c r="D24" t="str">
-        <f>RIGHT(A24,9)</f>
+        <f t="shared" si="0"/>
         <v>362489100</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>23293814619</v>
       </c>
@@ -712,11 +735,11 @@
         <v>24</v>
       </c>
       <c r="D25" t="str">
-        <f>RIGHT(A25,9)</f>
+        <f t="shared" si="0"/>
         <v>293814619</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>20365425532</v>
       </c>
@@ -724,11 +747,11 @@
         <v>25</v>
       </c>
       <c r="D26" t="str">
-        <f>RIGHT(A26,9)</f>
+        <f t="shared" si="0"/>
         <v>365425532</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>27316378035</v>
       </c>
@@ -736,11 +759,11 @@
         <v>26</v>
       </c>
       <c r="D27" t="str">
-        <f>RIGHT(A27,9)</f>
+        <f t="shared" si="0"/>
         <v>316378035</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>23273174524</v>
       </c>
@@ -748,11 +771,11 @@
         <v>27</v>
       </c>
       <c r="D28" t="str">
-        <f>RIGHT(A28,9)</f>
+        <f t="shared" si="0"/>
         <v>273174524</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>20364406321</v>
       </c>
@@ -760,11 +783,11 @@
         <v>28</v>
       </c>
       <c r="D29" t="str">
-        <f>RIGHT(A29,9)</f>
+        <f t="shared" si="0"/>
         <v>364406321</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>27253962793</v>
       </c>
@@ -772,11 +795,11 @@
         <v>29</v>
       </c>
       <c r="D30" t="str">
-        <f>RIGHT(A30,9)</f>
+        <f t="shared" si="0"/>
         <v>253962793</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>20236286534</v>
       </c>
@@ -784,11 +807,11 @@
         <v>30</v>
       </c>
       <c r="D31" t="str">
-        <f>RIGHT(A31,9)</f>
+        <f t="shared" si="0"/>
         <v>236286534</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>20354983452</v>
       </c>
@@ -796,11 +819,11 @@
         <v>31</v>
       </c>
       <c r="D32" t="str">
-        <f>RIGHT(A32,9)</f>
+        <f t="shared" si="0"/>
         <v>354983452</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>27304485782</v>
       </c>
@@ -808,11 +831,11 @@
         <v>32</v>
       </c>
       <c r="D33" t="str">
-        <f>RIGHT(A33,9)</f>
+        <f t="shared" si="0"/>
         <v>304485782</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34">
         <v>27222252992</v>
       </c>
@@ -820,11 +843,11 @@
         <v>33</v>
       </c>
       <c r="D34" t="str">
-        <f>RIGHT(A34,9)</f>
+        <f t="shared" ref="D34:D65" si="1">RIGHT(A34,9)</f>
         <v>222252992</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35">
         <v>27376670460</v>
       </c>
@@ -832,11 +855,11 @@
         <v>34</v>
       </c>
       <c r="D35" t="str">
-        <f>RIGHT(A35,9)</f>
+        <f t="shared" si="1"/>
         <v>376670460</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36">
         <v>27206365043</v>
       </c>
@@ -844,11 +867,11 @@
         <v>35</v>
       </c>
       <c r="D36" t="str">
-        <f>RIGHT(A36,9)</f>
+        <f t="shared" si="1"/>
         <v>206365043</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37">
         <v>20364007532</v>
       </c>
@@ -856,11 +879,11 @@
         <v>36</v>
       </c>
       <c r="D37" t="str">
-        <f>RIGHT(A37,9)</f>
+        <f t="shared" si="1"/>
         <v>364007532</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38">
         <v>20346437546</v>
       </c>
@@ -868,11 +891,11 @@
         <v>37</v>
       </c>
       <c r="D38" t="str">
-        <f>RIGHT(A38,9)</f>
+        <f t="shared" si="1"/>
         <v>346437546</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39">
         <v>20343945699</v>
       </c>
@@ -880,11 +903,11 @@
         <v>38</v>
       </c>
       <c r="D39" t="str">
-        <f>RIGHT(A39,9)</f>
+        <f t="shared" si="1"/>
         <v>343945699</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40">
         <v>27374268819</v>
       </c>
@@ -892,11 +915,11 @@
         <v>39</v>
       </c>
       <c r="D40" t="str">
-        <f>RIGHT(A40,9)</f>
+        <f t="shared" si="1"/>
         <v>374268819</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="A41">
         <v>20367271737</v>
       </c>
@@ -904,11 +927,11 @@
         <v>40</v>
       </c>
       <c r="D41" t="str">
-        <f>RIGHT(A41,9)</f>
+        <f t="shared" si="1"/>
         <v>367271737</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42">
         <v>20281965477</v>
       </c>
@@ -916,11 +939,11 @@
         <v>41</v>
       </c>
       <c r="D42" t="str">
-        <f>RIGHT(A42,9)</f>
+        <f t="shared" si="1"/>
         <v>281965477</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43">
         <v>23268636889</v>
       </c>
@@ -928,11 +951,11 @@
         <v>42</v>
       </c>
       <c r="D43" t="str">
-        <f>RIGHT(A43,9)</f>
+        <f t="shared" si="1"/>
         <v>268636889</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44">
         <v>20358024115</v>
       </c>
@@ -940,11 +963,11 @@
         <v>43</v>
       </c>
       <c r="D44" t="str">
-        <f>RIGHT(A44,9)</f>
+        <f t="shared" si="1"/>
         <v>358024115</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="A45">
         <v>27350683610</v>
       </c>
@@ -952,11 +975,11 @@
         <v>44</v>
       </c>
       <c r="D45" t="str">
-        <f>RIGHT(A45,9)</f>
+        <f t="shared" si="1"/>
         <v>350683610</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="A46">
         <v>27288436342</v>
       </c>
@@ -964,11 +987,11 @@
         <v>45</v>
       </c>
       <c r="D46" t="str">
-        <f>RIGHT(A46,9)</f>
+        <f t="shared" si="1"/>
         <v>288436342</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="A47">
         <v>27939993679</v>
       </c>
@@ -976,11 +999,11 @@
         <v>46</v>
       </c>
       <c r="D47" t="str">
-        <f>RIGHT(A47,9)</f>
+        <f t="shared" si="1"/>
         <v>939993679</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="A48">
         <v>27352024843</v>
       </c>
@@ -988,11 +1011,11 @@
         <v>47</v>
       </c>
       <c r="D48" t="str">
-        <f>RIGHT(A48,9)</f>
+        <f t="shared" si="1"/>
         <v>352024843</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="A49">
         <v>27291739518</v>
       </c>
@@ -1000,11 +1023,11 @@
         <v>48</v>
       </c>
       <c r="D49" t="str">
-        <f>RIGHT(A49,9)</f>
+        <f t="shared" si="1"/>
         <v>291739518</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="A50">
         <v>27290076434</v>
       </c>
@@ -1012,11 +1035,11 @@
         <v>49</v>
       </c>
       <c r="D50" t="str">
-        <f>RIGHT(A50,9)</f>
+        <f t="shared" si="1"/>
         <v>290076434</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4">
       <c r="A51">
         <v>27376096756</v>
       </c>
@@ -1024,11 +1047,11 @@
         <v>50</v>
       </c>
       <c r="D51" t="str">
-        <f>RIGHT(A51,9)</f>
+        <f t="shared" si="1"/>
         <v>376096756</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4">
       <c r="A52">
         <v>20164920217</v>
       </c>
@@ -1036,11 +1059,11 @@
         <v>51</v>
       </c>
       <c r="D52" t="str">
-        <f>RIGHT(A52,9)</f>
+        <f t="shared" si="1"/>
         <v>164920217</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4">
       <c r="A53">
         <v>27359602435</v>
       </c>
@@ -1048,11 +1071,11 @@
         <v>52</v>
       </c>
       <c r="D53" t="str">
-        <f>RIGHT(A53,9)</f>
+        <f t="shared" si="1"/>
         <v>359602435</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4">
       <c r="A54">
         <v>20346007924</v>
       </c>
@@ -1060,11 +1083,11 @@
         <v>53</v>
       </c>
       <c r="D54" t="str">
-        <f>RIGHT(A54,9)</f>
+        <f t="shared" si="1"/>
         <v>346007924</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4">
       <c r="A55">
         <v>27359952347</v>
       </c>
@@ -1072,11 +1095,11 @@
         <v>54</v>
       </c>
       <c r="D55" t="str">
-        <f>RIGHT(A55,9)</f>
+        <f t="shared" si="1"/>
         <v>359952347</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4">
       <c r="A56">
         <v>27361646806</v>
       </c>
@@ -1084,11 +1107,11 @@
         <v>55</v>
       </c>
       <c r="D56" t="str">
-        <f>RIGHT(A56,9)</f>
+        <f t="shared" si="1"/>
         <v>361646806</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4">
       <c r="A57">
         <v>20286408401</v>
       </c>
@@ -1096,11 +1119,11 @@
         <v>56</v>
       </c>
       <c r="D57" t="str">
-        <f>RIGHT(A57,9)</f>
+        <f t="shared" si="1"/>
         <v>286408401</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4">
       <c r="A58">
         <v>27342620006</v>
       </c>
@@ -1108,11 +1131,11 @@
         <v>57</v>
       </c>
       <c r="D58" t="str">
-        <f>RIGHT(A58,9)</f>
+        <f t="shared" si="1"/>
         <v>342620006</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4">
       <c r="A59">
         <v>20271204893</v>
       </c>
@@ -1120,11 +1143,11 @@
         <v>58</v>
       </c>
       <c r="D59" t="str">
-        <f>RIGHT(A59,9)</f>
+        <f t="shared" si="1"/>
         <v>271204893</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4">
       <c r="A60">
         <v>20353809580</v>
       </c>
@@ -1132,11 +1155,11 @@
         <v>59</v>
       </c>
       <c r="D60" t="str">
-        <f>RIGHT(A60,9)</f>
+        <f t="shared" si="1"/>
         <v>353809580</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4">
       <c r="A61">
         <v>27378411691</v>
       </c>
@@ -1144,11 +1167,11 @@
         <v>60</v>
       </c>
       <c r="D61" t="str">
-        <f>RIGHT(A61,9)</f>
+        <f t="shared" si="1"/>
         <v>378411691</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4">
       <c r="A62">
         <v>27279419990</v>
       </c>
@@ -1156,11 +1179,11 @@
         <v>61</v>
       </c>
       <c r="D62" t="str">
-        <f>RIGHT(A62,9)</f>
+        <f t="shared" si="1"/>
         <v>279419990</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4">
       <c r="A63">
         <v>27321099306</v>
       </c>
@@ -1168,11 +1191,11 @@
         <v>62</v>
       </c>
       <c r="D63" t="str">
-        <f>RIGHT(A63,9)</f>
+        <f t="shared" si="1"/>
         <v>321099306</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4">
       <c r="A64">
         <v>27356032786</v>
       </c>
@@ -1180,11 +1203,11 @@
         <v>63</v>
       </c>
       <c r="D64" t="str">
-        <f>RIGHT(A64,9)</f>
+        <f t="shared" si="1"/>
         <v>356032786</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4">
       <c r="A65">
         <v>20286643931</v>
       </c>
@@ -1192,11 +1215,11 @@
         <v>64</v>
       </c>
       <c r="D65" t="str">
-        <f>RIGHT(A65,9)</f>
+        <f t="shared" si="1"/>
         <v>286643931</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4">
       <c r="A66">
         <v>27264364952</v>
       </c>
@@ -1204,11 +1227,11 @@
         <v>65</v>
       </c>
       <c r="D66" t="str">
-        <f>RIGHT(A66,9)</f>
+        <f t="shared" ref="D66:D101" si="2">RIGHT(A66,9)</f>
         <v>264364952</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4">
       <c r="A67">
         <v>20358639802</v>
       </c>
@@ -1216,11 +1239,11 @@
         <v>66</v>
       </c>
       <c r="D67" t="str">
-        <f>RIGHT(A67,9)</f>
+        <f t="shared" si="2"/>
         <v>358639802</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4">
       <c r="A68">
         <v>20345134108</v>
       </c>
@@ -1228,11 +1251,11 @@
         <v>67</v>
       </c>
       <c r="D68" t="str">
-        <f>RIGHT(A68,9)</f>
+        <f t="shared" si="2"/>
         <v>345134108</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4">
       <c r="A69">
         <v>27333477268</v>
       </c>
@@ -1240,11 +1263,11 @@
         <v>68</v>
       </c>
       <c r="D69" t="str">
-        <f>RIGHT(A69,9)</f>
+        <f t="shared" si="2"/>
         <v>333477268</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4">
       <c r="A70">
         <v>27223510871</v>
       </c>
@@ -1252,11 +1275,11 @@
         <v>69</v>
       </c>
       <c r="D70" t="str">
-        <f>RIGHT(A70,9)</f>
+        <f t="shared" si="2"/>
         <v>223510871</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4">
       <c r="A71">
         <v>24270617391</v>
       </c>
@@ -1264,11 +1287,11 @@
         <v>70</v>
       </c>
       <c r="D71" t="str">
-        <f>RIGHT(A71,9)</f>
+        <f t="shared" si="2"/>
         <v>270617391</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4">
       <c r="A72">
         <v>23238768799</v>
       </c>
@@ -1276,11 +1299,11 @@
         <v>71</v>
       </c>
       <c r="D72" t="str">
-        <f>RIGHT(A72,9)</f>
+        <f t="shared" si="2"/>
         <v>238768799</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4">
       <c r="A73">
         <v>20268365886</v>
       </c>
@@ -1288,11 +1311,11 @@
         <v>72</v>
       </c>
       <c r="D73" t="str">
-        <f>RIGHT(A73,9)</f>
+        <f t="shared" si="2"/>
         <v>268365886</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4">
       <c r="A74">
         <v>23321861199</v>
       </c>
@@ -1300,11 +1323,11 @@
         <v>73</v>
       </c>
       <c r="D74" t="str">
-        <f>RIGHT(A74,9)</f>
+        <f t="shared" si="2"/>
         <v>321861199</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4">
       <c r="A75">
         <v>20261192404</v>
       </c>
@@ -1312,11 +1335,11 @@
         <v>74</v>
       </c>
       <c r="D75" t="str">
-        <f>RIGHT(A75,9)</f>
+        <f t="shared" si="2"/>
         <v>261192404</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4">
       <c r="A76">
         <v>23947259199</v>
       </c>
@@ -1324,11 +1347,11 @@
         <v>75</v>
       </c>
       <c r="D76" t="str">
-        <f>RIGHT(A76,9)</f>
+        <f t="shared" si="2"/>
         <v>947259199</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4">
       <c r="A77">
         <v>27246893387</v>
       </c>
@@ -1336,11 +1359,11 @@
         <v>76</v>
       </c>
       <c r="D77" t="str">
-        <f>RIGHT(A77,9)</f>
+        <f t="shared" si="2"/>
         <v>246893387</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4">
       <c r="A78">
         <v>27383455141</v>
       </c>
@@ -1348,11 +1371,11 @@
         <v>77</v>
       </c>
       <c r="D78" t="str">
-        <f>RIGHT(A78,9)</f>
+        <f t="shared" si="2"/>
         <v>383455141</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4">
       <c r="A79">
         <v>20364042184</v>
       </c>
@@ -1360,11 +1383,11 @@
         <v>78</v>
       </c>
       <c r="D79" t="str">
-        <f>RIGHT(A79,9)</f>
+        <f t="shared" si="2"/>
         <v>364042184</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4">
       <c r="A80">
         <v>20321115994</v>
       </c>
@@ -1372,11 +1395,11 @@
         <v>79</v>
       </c>
       <c r="D80" t="str">
-        <f>RIGHT(A80,9)</f>
+        <f t="shared" si="2"/>
         <v>321115994</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4">
       <c r="A81">
         <v>20345069411</v>
       </c>
@@ -1384,11 +1407,11 @@
         <v>80</v>
       </c>
       <c r="D81" t="str">
-        <f>RIGHT(A81,9)</f>
+        <f t="shared" si="2"/>
         <v>345069411</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4">
       <c r="A82">
         <v>27344381947</v>
       </c>
@@ -1396,11 +1419,11 @@
         <v>81</v>
       </c>
       <c r="D82" t="str">
-        <f>RIGHT(A82,9)</f>
+        <f t="shared" si="2"/>
         <v>344381947</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4">
       <c r="A83">
         <v>27334017279</v>
       </c>
@@ -1408,11 +1431,11 @@
         <v>82</v>
       </c>
       <c r="D83" t="str">
-        <f>RIGHT(A83,9)</f>
+        <f t="shared" si="2"/>
         <v>334017279</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4">
       <c r="A84">
         <v>27316253496</v>
       </c>
@@ -1420,11 +1443,11 @@
         <v>83</v>
       </c>
       <c r="D84" t="str">
-        <f>RIGHT(A84,9)</f>
+        <f t="shared" si="2"/>
         <v>316253496</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4">
       <c r="A85">
         <v>20331921557</v>
       </c>
@@ -1432,11 +1455,11 @@
         <v>84</v>
       </c>
       <c r="D85" t="str">
-        <f>RIGHT(A85,9)</f>
+        <f t="shared" si="2"/>
         <v>331921557</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4">
       <c r="A86">
         <v>20239652862</v>
       </c>
@@ -1444,11 +1467,11 @@
         <v>85</v>
       </c>
       <c r="D86" t="str">
-        <f>RIGHT(A86,9)</f>
+        <f t="shared" si="2"/>
         <v>239652862</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4">
       <c r="A87">
         <v>27305909756</v>
       </c>
@@ -1456,11 +1479,11 @@
         <v>86</v>
       </c>
       <c r="D87" t="str">
-        <f>RIGHT(A87,9)</f>
+        <f t="shared" si="2"/>
         <v>305909756</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4">
       <c r="A88">
         <v>23294616349</v>
       </c>
@@ -1468,11 +1491,11 @@
         <v>87</v>
       </c>
       <c r="D88" t="str">
-        <f>RIGHT(A88,9)</f>
+        <f t="shared" si="2"/>
         <v>294616349</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4">
       <c r="A89">
         <v>23304494964</v>
       </c>
@@ -1480,11 +1503,11 @@
         <v>88</v>
       </c>
       <c r="D89" t="str">
-        <f>RIGHT(A89,9)</f>
+        <f t="shared" si="2"/>
         <v>304494964</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4">
       <c r="A90">
         <v>20359422548</v>
       </c>
@@ -1492,11 +1515,11 @@
         <v>89</v>
       </c>
       <c r="D90" t="str">
-        <f>RIGHT(A90,9)</f>
+        <f t="shared" si="2"/>
         <v>359422548</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4">
       <c r="A91">
         <v>27297037221</v>
       </c>
@@ -1504,11 +1527,11 @@
         <v>90</v>
       </c>
       <c r="D91" t="str">
-        <f>RIGHT(A91,9)</f>
+        <f t="shared" si="2"/>
         <v>297037221</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4">
       <c r="A92">
         <v>27363985780</v>
       </c>
@@ -1516,11 +1539,11 @@
         <v>91</v>
       </c>
       <c r="D92" t="str">
-        <f>RIGHT(A92,9)</f>
+        <f t="shared" si="2"/>
         <v>363985780</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4">
       <c r="A93">
         <v>20252316117</v>
       </c>
@@ -1528,11 +1551,11 @@
         <v>92</v>
       </c>
       <c r="D93" t="str">
-        <f>RIGHT(A93,9)</f>
+        <f t="shared" si="2"/>
         <v>252316117</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4">
       <c r="A94">
         <v>20939221442</v>
       </c>
@@ -1540,11 +1563,11 @@
         <v>93</v>
       </c>
       <c r="D94" t="str">
-        <f>RIGHT(A94,9)</f>
+        <f t="shared" si="2"/>
         <v>939221442</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4">
       <c r="A95">
         <v>20286925732</v>
       </c>
@@ -1552,11 +1575,11 @@
         <v>94</v>
       </c>
       <c r="D95" t="str">
-        <f>RIGHT(A95,9)</f>
+        <f t="shared" si="2"/>
         <v>286925732</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4">
       <c r="A96">
         <v>20331547949</v>
       </c>
@@ -1564,11 +1587,11 @@
         <v>95</v>
       </c>
       <c r="D96" t="str">
-        <f>RIGHT(A96,9)</f>
+        <f t="shared" si="2"/>
         <v>331547949</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4">
       <c r="A97">
         <v>20236728618</v>
       </c>
@@ -1576,11 +1599,11 @@
         <v>96</v>
       </c>
       <c r="D97" t="str">
-        <f>RIGHT(A97,9)</f>
+        <f t="shared" si="2"/>
         <v>236728618</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4">
       <c r="A98">
         <v>23372162244</v>
       </c>
@@ -1588,11 +1611,11 @@
         <v>97</v>
       </c>
       <c r="D98" t="str">
-        <f>RIGHT(A98,9)</f>
+        <f t="shared" si="2"/>
         <v>372162244</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4">
       <c r="A99">
         <v>27271812677</v>
       </c>
@@ -1600,11 +1623,11 @@
         <v>98</v>
       </c>
       <c r="D99" t="str">
-        <f>RIGHT(A99,9)</f>
+        <f t="shared" si="2"/>
         <v>271812677</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4">
       <c r="A100">
         <v>20263715412</v>
       </c>
@@ -1612,11 +1635,11 @@
         <v>99</v>
       </c>
       <c r="D100" t="str">
-        <f>RIGHT(A100,9)</f>
+        <f t="shared" si="2"/>
         <v>263715412</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4">
       <c r="A101">
         <v>27351695701</v>
       </c>
@@ -1624,29 +1647,33 @@
         <v>100</v>
       </c>
       <c r="D101" t="str">
-        <f>RIGHT(A101,9)</f>
+        <f t="shared" si="2"/>
         <v>351695701</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A101">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A102" sqref="A102:A201"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1654,923 +1681,1632 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="str">
-        <f>LEFT(Hoja1!D2,9)</f>
-        <v>324717928</v>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>32096467</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="str">
-        <f>LEFT(Hoja1!D3,9)</f>
-        <v>289070406</v>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>20647870</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="str">
-        <f>LEFT(Hoja1!D4,9)</f>
-        <v>325850820</v>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>20347118</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="str">
-        <f>LEFT(Hoja1!D5,9)</f>
-        <v>288183784</v>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>25574544</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="str">
-        <f>LEFT(Hoja1!D6,9)</f>
-        <v>303681329</v>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>29585676</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="str">
-        <f>LEFT(Hoja1!D7,9)</f>
-        <v>328919249</v>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>26868305</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="str">
-        <f>LEFT(Hoja1!D8,9)</f>
-        <v>272593103</v>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>19980772</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="str">
-        <f>LEFT(Hoja1!D9,9)</f>
-        <v>381688599</v>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>24686460</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="str">
-        <f>LEFT(Hoja1!D10,9)</f>
-        <v>222764114</v>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>22554028</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="str">
-        <f>LEFT(Hoja1!D11,9)</f>
-        <v>345916453</v>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>19245391</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="str">
-        <f>LEFT(Hoja1!D12,9)</f>
-        <v>376091029</v>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>18041182</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="str">
-        <f>LEFT(Hoja1!D13,9)</f>
-        <v>309349369</v>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>25167480</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="str">
-        <f>LEFT(Hoja1!D14,9)</f>
-        <v>378054002</v>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>21285840</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="str">
-        <f>LEFT(Hoja1!D15,9)</f>
-        <v>330368921</v>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>27520532</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="str">
-        <f>LEFT(Hoja1!D16,9)</f>
-        <v>363593475</v>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>24572930</v>
       </c>
       <c r="B16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="str">
-        <f>LEFT(Hoja1!D17,9)</f>
-        <v>366906369</v>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>34557321</v>
       </c>
       <c r="B17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="str">
-        <f>LEFT(Hoja1!D18,9)</f>
-        <v>275355535</v>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>29795794</v>
       </c>
       <c r="B18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="str">
-        <f>LEFT(Hoja1!D19,9)</f>
-        <v>366027926</v>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>21640394</v>
       </c>
       <c r="B19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="str">
-        <f>LEFT(Hoja1!D20,9)</f>
-        <v>315410970</v>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>31657842</v>
       </c>
       <c r="B20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="str">
-        <f>LEFT(Hoja1!D21,9)</f>
-        <v>309145802</v>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>18944096</v>
       </c>
       <c r="B21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="str">
-        <f>LEFT(Hoja1!D22,9)</f>
-        <v>365973720</v>
+    <row r="22" spans="1:2">
+      <c r="A22">
+        <v>31965824</v>
       </c>
       <c r="B22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="str">
-        <f>LEFT(Hoja1!D23,9)</f>
-        <v>259702349</v>
+    <row r="23" spans="1:2">
+      <c r="A23">
+        <v>17592277</v>
       </c>
       <c r="B23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="str">
-        <f>LEFT(Hoja1!D24,9)</f>
-        <v>362489100</v>
+    <row r="24" spans="1:2">
+      <c r="A24">
+        <v>21814714</v>
       </c>
       <c r="B24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="str">
-        <f>LEFT(Hoja1!D25,9)</f>
-        <v>293814619</v>
+    <row r="25" spans="1:2">
+      <c r="A25">
+        <v>18131354</v>
       </c>
       <c r="B25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="str">
-        <f>LEFT(Hoja1!D26,9)</f>
-        <v>365425532</v>
+    <row r="26" spans="1:2">
+      <c r="A26">
+        <v>24316104</v>
       </c>
       <c r="B26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="str">
-        <f>LEFT(Hoja1!D27,9)</f>
-        <v>316378035</v>
+    <row r="27" spans="1:2">
+      <c r="A27">
+        <v>34974848</v>
       </c>
       <c r="B27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="str">
-        <f>LEFT(Hoja1!D28,9)</f>
-        <v>273174524</v>
+    <row r="28" spans="1:2">
+      <c r="A28">
+        <v>18837447</v>
       </c>
       <c r="B28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="str">
-        <f>LEFT(Hoja1!D29,9)</f>
-        <v>364406321</v>
+    <row r="29" spans="1:2">
+      <c r="A29">
+        <v>27047705</v>
       </c>
       <c r="B29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="str">
-        <f>LEFT(Hoja1!D30,9)</f>
-        <v>253962793</v>
+    <row r="30" spans="1:2">
+      <c r="A30">
+        <v>24589925</v>
       </c>
       <c r="B30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="str">
-        <f>LEFT(Hoja1!D31,9)</f>
-        <v>236286534</v>
+    <row r="31" spans="1:2">
+      <c r="A31">
+        <v>26845383</v>
       </c>
       <c r="B31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="str">
-        <f>LEFT(Hoja1!D32,9)</f>
-        <v>354983452</v>
+    <row r="32" spans="1:2">
+      <c r="A32">
+        <v>27703543</v>
       </c>
       <c r="B32">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="str">
-        <f>LEFT(Hoja1!D33,9)</f>
-        <v>304485782</v>
+    <row r="33" spans="1:2">
+      <c r="A33">
+        <v>25489762</v>
       </c>
       <c r="B33">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="str">
-        <f>LEFT(Hoja1!D34,9)</f>
-        <v>222252992</v>
+    <row r="34" spans="1:2">
+      <c r="A34">
+        <v>19036988</v>
       </c>
       <c r="B34">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="str">
-        <f>LEFT(Hoja1!D35,9)</f>
-        <v>376670460</v>
+    <row r="35" spans="1:2">
+      <c r="A35">
+        <v>15755794</v>
       </c>
       <c r="B35">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="str">
-        <f>LEFT(Hoja1!D36,9)</f>
-        <v>206365043</v>
+    <row r="36" spans="1:2">
+      <c r="A36">
+        <v>20897843</v>
       </c>
       <c r="B36">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="str">
-        <f>LEFT(Hoja1!D37,9)</f>
-        <v>364007532</v>
+    <row r="37" spans="1:2">
+      <c r="A37">
+        <v>34239679</v>
       </c>
       <c r="B37">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="str">
-        <f>LEFT(Hoja1!D38,9)</f>
-        <v>346437546</v>
+    <row r="38" spans="1:2">
+      <c r="A38">
+        <v>26551089</v>
       </c>
       <c r="B38">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="str">
-        <f>LEFT(Hoja1!D39,9)</f>
-        <v>343945699</v>
+    <row r="39" spans="1:2">
+      <c r="A39">
+        <v>18557593</v>
       </c>
       <c r="B39">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="str">
-        <f>LEFT(Hoja1!D40,9)</f>
-        <v>374268819</v>
+    <row r="40" spans="1:2">
+      <c r="A40">
+        <v>25098867</v>
       </c>
       <c r="B40">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="str">
-        <f>LEFT(Hoja1!D41,9)</f>
-        <v>367271737</v>
+    <row r="41" spans="1:2">
+      <c r="A41">
+        <v>27604761</v>
       </c>
       <c r="B41">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="str">
-        <f>LEFT(Hoja1!D42,9)</f>
-        <v>281965477</v>
+    <row r="42" spans="1:2">
+      <c r="A42">
+        <v>25581528</v>
       </c>
       <c r="B42">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="str">
-        <f>LEFT(Hoja1!D43,9)</f>
-        <v>268636889</v>
+    <row r="43" spans="1:2">
+      <c r="A43">
+        <v>32837992</v>
       </c>
       <c r="B43">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="str">
-        <f>LEFT(Hoja1!D44,9)</f>
-        <v>358024115</v>
+    <row r="44" spans="1:2">
+      <c r="A44">
+        <v>29042728</v>
       </c>
       <c r="B44">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="str">
-        <f>LEFT(Hoja1!D45,9)</f>
-        <v>350683610</v>
+    <row r="45" spans="1:2">
+      <c r="A45">
+        <v>23389737</v>
       </c>
       <c r="B45">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="str">
-        <f>LEFT(Hoja1!D46,9)</f>
-        <v>288436342</v>
+    <row r="46" spans="1:2">
+      <c r="A46">
+        <v>23187345</v>
       </c>
       <c r="B46">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="str">
-        <f>LEFT(Hoja1!D47,9)</f>
-        <v>939993679</v>
+    <row r="47" spans="1:2">
+      <c r="A47">
+        <v>27942195</v>
       </c>
       <c r="B47">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="str">
-        <f>LEFT(Hoja1!D48,9)</f>
-        <v>352024843</v>
+    <row r="48" spans="1:2">
+      <c r="A48">
+        <v>31152632</v>
       </c>
       <c r="B48">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="str">
-        <f>LEFT(Hoja1!D49,9)</f>
-        <v>291739518</v>
+    <row r="49" spans="1:2">
+      <c r="A49">
+        <v>15969214</v>
       </c>
       <c r="B49">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="str">
-        <f>LEFT(Hoja1!D50,9)</f>
-        <v>290076434</v>
+    <row r="50" spans="1:2">
+      <c r="A50">
+        <v>30976043</v>
       </c>
       <c r="B50">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="str">
-        <f>LEFT(Hoja1!D51,9)</f>
-        <v>376096756</v>
+    <row r="51" spans="1:2">
+      <c r="A51">
+        <v>24672474</v>
       </c>
       <c r="B51">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="str">
-        <f>LEFT(Hoja1!D52,9)</f>
-        <v>164920217</v>
+    <row r="52" spans="1:2">
+      <c r="A52">
+        <v>24642604</v>
       </c>
       <c r="B52">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="str">
-        <f>LEFT(Hoja1!D53,9)</f>
-        <v>359602435</v>
+    <row r="53" spans="1:2">
+      <c r="A53">
+        <v>31642295</v>
       </c>
       <c r="B53">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="str">
-        <f>LEFT(Hoja1!D54,9)</f>
-        <v>346007924</v>
+    <row r="54" spans="1:2">
+      <c r="A54">
+        <v>27529809</v>
       </c>
       <c r="B54">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="str">
-        <f>LEFT(Hoja1!D55,9)</f>
-        <v>359952347</v>
+    <row r="55" spans="1:2">
+      <c r="A55">
+        <v>24262103</v>
       </c>
       <c r="B55">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="str">
-        <f>LEFT(Hoja1!D56,9)</f>
-        <v>361646806</v>
+    <row r="56" spans="1:2">
+      <c r="A56">
+        <v>22207525</v>
       </c>
       <c r="B56">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="str">
-        <f>LEFT(Hoja1!D57,9)</f>
-        <v>286408401</v>
+    <row r="57" spans="1:2">
+      <c r="A57">
+        <v>16187044</v>
       </c>
       <c r="B57">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="str">
-        <f>LEFT(Hoja1!D58,9)</f>
-        <v>342620006</v>
+    <row r="58" spans="1:2">
+      <c r="A58">
+        <v>25153656</v>
       </c>
       <c r="B58">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="str">
-        <f>LEFT(Hoja1!D59,9)</f>
-        <v>271204893</v>
+    <row r="59" spans="1:2">
+      <c r="A59">
+        <v>17985423</v>
       </c>
       <c r="B59">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="str">
-        <f>LEFT(Hoja1!D60,9)</f>
-        <v>353809580</v>
+    <row r="60" spans="1:2">
+      <c r="A60">
+        <v>30641872</v>
       </c>
       <c r="B60">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="str">
-        <f>LEFT(Hoja1!D61,9)</f>
-        <v>378411691</v>
+    <row r="61" spans="1:2">
+      <c r="A61">
+        <v>18839338</v>
       </c>
       <c r="B61">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="str">
-        <f>LEFT(Hoja1!D62,9)</f>
-        <v>279419990</v>
+    <row r="62" spans="1:2">
+      <c r="A62">
+        <v>31473787</v>
       </c>
       <c r="B62">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="str">
-        <f>LEFT(Hoja1!D63,9)</f>
-        <v>321099306</v>
+    <row r="63" spans="1:2">
+      <c r="A63">
+        <v>28558962</v>
       </c>
       <c r="B63">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="str">
-        <f>LEFT(Hoja1!D64,9)</f>
-        <v>356032786</v>
+    <row r="64" spans="1:2">
+      <c r="A64">
+        <v>17923094</v>
       </c>
       <c r="B64">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="str">
-        <f>LEFT(Hoja1!D65,9)</f>
-        <v>286643931</v>
+    <row r="65" spans="1:2">
+      <c r="A65">
+        <v>34358608</v>
       </c>
       <c r="B65">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="str">
-        <f>LEFT(Hoja1!D66,9)</f>
-        <v>264364952</v>
+    <row r="66" spans="1:2">
+      <c r="A66">
+        <v>21878506</v>
       </c>
       <c r="B66">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="str">
-        <f>LEFT(Hoja1!D67,9)</f>
-        <v>358639802</v>
+    <row r="67" spans="1:2">
+      <c r="A67">
+        <v>17048816</v>
       </c>
       <c r="B67">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="str">
-        <f>LEFT(Hoja1!D68,9)</f>
-        <v>345134108</v>
+    <row r="68" spans="1:2">
+      <c r="A68">
+        <v>32253538</v>
       </c>
       <c r="B68">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" t="str">
-        <f>LEFT(Hoja1!D69,9)</f>
-        <v>333477268</v>
+    <row r="69" spans="1:2">
+      <c r="A69">
+        <v>25203547</v>
       </c>
       <c r="B69">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" t="str">
-        <f>LEFT(Hoja1!D70,9)</f>
-        <v>223510871</v>
+    <row r="70" spans="1:2">
+      <c r="A70">
+        <v>33028506</v>
       </c>
       <c r="B70">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="str">
-        <f>LEFT(Hoja1!D71,9)</f>
-        <v>270617391</v>
+    <row r="71" spans="1:2">
+      <c r="A71">
+        <v>31656189</v>
       </c>
       <c r="B71">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" t="str">
-        <f>LEFT(Hoja1!D72,9)</f>
-        <v>238768799</v>
+    <row r="72" spans="1:2">
+      <c r="A72">
+        <v>24463672</v>
       </c>
       <c r="B72">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="str">
-        <f>LEFT(Hoja1!D73,9)</f>
-        <v>268365886</v>
+    <row r="73" spans="1:2">
+      <c r="A73">
+        <v>16940172</v>
       </c>
       <c r="B73">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" t="str">
-        <f>LEFT(Hoja1!D74,9)</f>
-        <v>321861199</v>
+    <row r="74" spans="1:2">
+      <c r="A74">
+        <v>24149517</v>
       </c>
       <c r="B74">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" t="str">
-        <f>LEFT(Hoja1!D75,9)</f>
-        <v>261192404</v>
+    <row r="75" spans="1:2">
+      <c r="A75">
+        <v>18920859</v>
       </c>
       <c r="B75">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" t="str">
-        <f>LEFT(Hoja1!D76,9)</f>
-        <v>947259199</v>
+    <row r="76" spans="1:2">
+      <c r="A76">
+        <v>27569447</v>
       </c>
       <c r="B76">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" t="str">
-        <f>LEFT(Hoja1!D77,9)</f>
-        <v>246893387</v>
+    <row r="77" spans="1:2">
+      <c r="A77">
+        <v>30925256</v>
       </c>
       <c r="B77">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" t="str">
-        <f>LEFT(Hoja1!D78,9)</f>
-        <v>383455141</v>
+    <row r="78" spans="1:2">
+      <c r="A78">
+        <v>30054231</v>
       </c>
       <c r="B78">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" t="str">
-        <f>LEFT(Hoja1!D79,9)</f>
-        <v>364042184</v>
+    <row r="79" spans="1:2">
+      <c r="A79">
+        <v>22166629</v>
       </c>
       <c r="B79">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" t="str">
-        <f>LEFT(Hoja1!D80,9)</f>
-        <v>321115994</v>
+    <row r="80" spans="1:2">
+      <c r="A80">
+        <v>19119398</v>
       </c>
       <c r="B80">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="str">
-        <f>LEFT(Hoja1!D81,9)</f>
-        <v>345069411</v>
+    <row r="81" spans="1:2">
+      <c r="A81">
+        <v>22673405</v>
       </c>
       <c r="B81">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" t="str">
-        <f>LEFT(Hoja1!D82,9)</f>
-        <v>344381947</v>
+    <row r="82" spans="1:2">
+      <c r="A82">
+        <v>28415922</v>
       </c>
       <c r="B82">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" t="str">
-        <f>LEFT(Hoja1!D83,9)</f>
-        <v>334017279</v>
+    <row r="83" spans="1:2">
+      <c r="A83">
+        <v>23622405</v>
       </c>
       <c r="B83">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" t="str">
-        <f>LEFT(Hoja1!D84,9)</f>
-        <v>316253496</v>
+    <row r="84" spans="1:2">
+      <c r="A84">
+        <v>33072109</v>
       </c>
       <c r="B84">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" t="str">
-        <f>LEFT(Hoja1!D85,9)</f>
-        <v>331921557</v>
+    <row r="85" spans="1:2">
+      <c r="A85">
+        <v>23421776</v>
       </c>
       <c r="B85">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" t="str">
-        <f>LEFT(Hoja1!D86,9)</f>
-        <v>239652862</v>
+    <row r="86" spans="1:2">
+      <c r="A86">
+        <v>26071335</v>
       </c>
       <c r="B86">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" t="str">
-        <f>LEFT(Hoja1!D87,9)</f>
-        <v>305909756</v>
+    <row r="87" spans="1:2">
+      <c r="A87">
+        <v>24263836</v>
       </c>
       <c r="B87">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" t="str">
-        <f>LEFT(Hoja1!D88,9)</f>
-        <v>294616349</v>
+    <row r="88" spans="1:2">
+      <c r="A88">
+        <v>19339218</v>
       </c>
       <c r="B88">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" t="str">
-        <f>LEFT(Hoja1!D89,9)</f>
-        <v>304494964</v>
+    <row r="89" spans="1:2">
+      <c r="A89">
+        <v>34837359</v>
       </c>
       <c r="B89">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" t="str">
-        <f>LEFT(Hoja1!D90,9)</f>
-        <v>359422548</v>
+    <row r="90" spans="1:2">
+      <c r="A90">
+        <v>18968297</v>
       </c>
       <c r="B90">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" t="str">
-        <f>LEFT(Hoja1!D91,9)</f>
-        <v>297037221</v>
+    <row r="91" spans="1:2">
+      <c r="A91">
+        <v>25381386</v>
       </c>
       <c r="B91">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" t="str">
-        <f>LEFT(Hoja1!D92,9)</f>
-        <v>363985780</v>
+    <row r="92" spans="1:2">
+      <c r="A92">
+        <v>32492863</v>
       </c>
       <c r="B92">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" t="str">
-        <f>LEFT(Hoja1!D93,9)</f>
-        <v>252316117</v>
+    <row r="93" spans="1:2">
+      <c r="A93">
+        <v>29050116</v>
       </c>
       <c r="B93">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" t="str">
-        <f>LEFT(Hoja1!D94,9)</f>
-        <v>939221442</v>
+    <row r="94" spans="1:2">
+      <c r="A94">
+        <v>32465702</v>
       </c>
       <c r="B94">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" t="str">
-        <f>LEFT(Hoja1!D95,9)</f>
-        <v>286925732</v>
+    <row r="95" spans="1:2">
+      <c r="A95">
+        <v>30487701</v>
       </c>
       <c r="B95">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" t="str">
-        <f>LEFT(Hoja1!D96,9)</f>
-        <v>331547949</v>
+    <row r="96" spans="1:2">
+      <c r="A96">
+        <v>33601679</v>
       </c>
       <c r="B96">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" t="str">
-        <f>LEFT(Hoja1!D97,9)</f>
-        <v>236728618</v>
+    <row r="97" spans="1:2">
+      <c r="A97">
+        <v>29810406</v>
       </c>
       <c r="B97">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" t="str">
-        <f>LEFT(Hoja1!D98,9)</f>
-        <v>372162244</v>
+    <row r="98" spans="1:2">
+      <c r="A98">
+        <v>15051339</v>
       </c>
       <c r="B98">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" t="str">
-        <f>LEFT(Hoja1!D99,9)</f>
-        <v>271812677</v>
+    <row r="99" spans="1:2">
+      <c r="A99">
+        <v>17133023</v>
       </c>
       <c r="B99">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" t="str">
-        <f>LEFT(Hoja1!D100,9)</f>
-        <v>263715412</v>
+    <row r="100" spans="1:2">
+      <c r="A100">
+        <v>20559239</v>
       </c>
       <c r="B100">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" t="str">
-        <f>LEFT(Hoja1!D101,9)</f>
-        <v>351695701</v>
+    <row r="101" spans="1:2">
+      <c r="A101">
+        <v>28910722</v>
       </c>
       <c r="B101">
         <v>100</v>
       </c>
     </row>
+    <row r="102" spans="1:2">
+      <c r="A102">
+        <v>26091292</v>
+      </c>
+      <c r="B102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103">
+        <v>22812890</v>
+      </c>
+      <c r="B103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104">
+        <v>27535553</v>
+      </c>
+      <c r="B104">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105">
+        <v>30914580</v>
+      </c>
+      <c r="B105">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106">
+        <v>24717521</v>
+      </c>
+      <c r="B106">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107">
+        <v>23628653</v>
+      </c>
+      <c r="B107">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108">
+        <v>30448578</v>
+      </c>
+      <c r="B108">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109">
+        <v>28196547</v>
+      </c>
+      <c r="B109">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110">
+        <v>16492021</v>
+      </c>
+      <c r="B110">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111">
+        <v>35380958</v>
+      </c>
+      <c r="B111">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112">
+        <v>22351087</v>
+      </c>
+      <c r="B112">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113">
+        <v>27061739</v>
+      </c>
+      <c r="B113">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114">
+        <v>23876879</v>
+      </c>
+      <c r="B114">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115">
+        <v>32111599</v>
+      </c>
+      <c r="B115">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116">
+        <v>30407599</v>
+      </c>
+      <c r="B116">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117">
+        <v>25231611</v>
+      </c>
+      <c r="B117">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118">
+        <v>23672861</v>
+      </c>
+      <c r="B118">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119">
+        <v>26756360</v>
+      </c>
+      <c r="B119">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120">
+        <v>24756508</v>
+      </c>
+      <c r="B120">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121">
+        <v>18545884</v>
+      </c>
+      <c r="B121">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122">
+        <v>24405970</v>
+      </c>
+      <c r="B122">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123">
+        <v>25370464</v>
+      </c>
+      <c r="B123">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124">
+        <v>32439727</v>
+      </c>
+      <c r="B124">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125">
+        <v>31937562</v>
+      </c>
+      <c r="B125">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126">
+        <v>30276531</v>
+      </c>
+      <c r="B126">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127">
+        <v>13348995</v>
+      </c>
+      <c r="B127">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128">
+        <v>35957660</v>
+      </c>
+      <c r="B128">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129">
+        <v>10000278</v>
+      </c>
+      <c r="B129">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130">
+        <v>26169317</v>
+      </c>
+      <c r="B130">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131">
+        <v>23413527</v>
+      </c>
+      <c r="B131">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132">
+        <v>26043475</v>
+      </c>
+      <c r="B132">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133">
+        <v>31292018</v>
+      </c>
+      <c r="B133">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134">
+        <v>24922379</v>
+      </c>
+      <c r="B134">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135">
+        <v>22288009</v>
+      </c>
+      <c r="B135">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136">
+        <v>22574668</v>
+      </c>
+      <c r="B136">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137">
+        <v>27284020</v>
+      </c>
+      <c r="B137">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138">
+        <v>93791921</v>
+      </c>
+      <c r="B138">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139">
+        <v>24336922</v>
+      </c>
+      <c r="B139">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140">
+        <v>32638727</v>
+      </c>
+      <c r="B140">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141">
+        <v>36403885</v>
+      </c>
+      <c r="B141">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142">
+        <v>31477190</v>
+      </c>
+      <c r="B142">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143">
+        <v>25182981</v>
+      </c>
+      <c r="B143">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144">
+        <v>26965196</v>
+      </c>
+      <c r="B144">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145">
+        <v>32091714</v>
+      </c>
+      <c r="B145">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146">
+        <v>30815197</v>
+      </c>
+      <c r="B146">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147">
+        <v>22666665</v>
+      </c>
+      <c r="B147">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148">
+        <v>29867735</v>
+      </c>
+      <c r="B148">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149">
+        <v>31752457</v>
+      </c>
+      <c r="B149">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150">
+        <v>29702373</v>
+      </c>
+      <c r="B150">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151">
+        <v>25847587</v>
+      </c>
+      <c r="B151">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152">
+        <v>20520064</v>
+      </c>
+      <c r="B152">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153">
+        <v>33017487</v>
+      </c>
+      <c r="B153">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154">
+        <v>21818154</v>
+      </c>
+      <c r="B154">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155">
+        <v>36921072</v>
+      </c>
+      <c r="B155">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156">
+        <v>22195367</v>
+      </c>
+      <c r="B156">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2">
+      <c r="A157">
+        <v>21972573</v>
+      </c>
+      <c r="B157">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2">
+      <c r="A158">
+        <v>26127463</v>
+      </c>
+      <c r="B158">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2">
+      <c r="A159">
+        <v>30934859</v>
+      </c>
+      <c r="B159">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
+      <c r="A160">
+        <v>26328066</v>
+      </c>
+      <c r="B160">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161">
+        <v>33391190</v>
+      </c>
+      <c r="B161">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2">
+      <c r="A162">
+        <v>27486398</v>
+      </c>
+      <c r="B162">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2">
+      <c r="A163">
+        <v>30410289</v>
+      </c>
+      <c r="B163">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2">
+      <c r="A164">
+        <v>27146494</v>
+      </c>
+      <c r="B164">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2">
+      <c r="A165">
+        <v>26387145</v>
+      </c>
+      <c r="B165">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2">
+      <c r="A166">
+        <v>26604529</v>
+      </c>
+      <c r="B166">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2">
+      <c r="A167">
+        <v>31963375</v>
+      </c>
+      <c r="B167">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2">
+      <c r="A168">
+        <v>27383550</v>
+      </c>
+      <c r="B168">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2">
+      <c r="A169">
+        <v>18808701</v>
+      </c>
+      <c r="B169">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2">
+      <c r="A170">
+        <v>25529423</v>
+      </c>
+      <c r="B170">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2">
+      <c r="A171">
+        <v>39664632</v>
+      </c>
+      <c r="B171">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2">
+      <c r="A172">
+        <v>25822174</v>
+      </c>
+      <c r="B172">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2">
+      <c r="A173">
+        <v>30218532</v>
+      </c>
+      <c r="B173">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2">
+      <c r="A174">
+        <v>29158026</v>
+      </c>
+      <c r="B174">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2">
+      <c r="A175">
+        <v>35122148</v>
+      </c>
+      <c r="B175">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2">
+      <c r="A176">
+        <v>32983368</v>
+      </c>
+      <c r="B176">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2">
+      <c r="A177">
+        <v>23050239</v>
+      </c>
+      <c r="B177">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2">
+      <c r="A178">
+        <v>94217792</v>
+      </c>
+      <c r="B178">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2">
+      <c r="A179">
+        <v>31929128</v>
+      </c>
+      <c r="B179">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2">
+      <c r="A180">
+        <v>18631066</v>
+      </c>
+      <c r="B180">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2">
+      <c r="A181">
+        <v>17726061</v>
+      </c>
+      <c r="B181">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2">
+      <c r="A182">
+        <v>25988906</v>
+      </c>
+      <c r="B182">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2">
+      <c r="A183">
+        <v>34519429</v>
+      </c>
+      <c r="B183">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2">
+      <c r="A184">
+        <v>25675517</v>
+      </c>
+      <c r="B184">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2">
+      <c r="A185">
+        <v>30586320</v>
+      </c>
+      <c r="B185">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2">
+      <c r="A186">
+        <v>29250659</v>
+      </c>
+      <c r="B186">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2">
+      <c r="A187">
+        <v>24905953</v>
+      </c>
+      <c r="B187">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2">
+      <c r="A188">
+        <v>31342470</v>
+      </c>
+      <c r="B188">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2">
+      <c r="A189">
+        <v>27152292</v>
+      </c>
+      <c r="B189">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2">
+      <c r="A190">
+        <v>33780102</v>
+      </c>
+      <c r="B190">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2">
+      <c r="A191">
+        <v>29799190</v>
+      </c>
+      <c r="B191">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2">
+      <c r="A192">
+        <v>36461022</v>
+      </c>
+      <c r="B192">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2">
+      <c r="A193">
+        <v>12683815</v>
+      </c>
+      <c r="B193">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2">
+      <c r="A194">
+        <v>36594138</v>
+      </c>
+      <c r="B194">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2">
+      <c r="A195">
+        <v>29906783</v>
+      </c>
+      <c r="B195">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2">
+      <c r="A196">
+        <v>36684361</v>
+      </c>
+      <c r="B196">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2">
+      <c r="A197">
+        <v>28825557</v>
+      </c>
+      <c r="B197">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2">
+      <c r="A198">
+        <v>35141683</v>
+      </c>
+      <c r="B198">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2">
+      <c r="A199">
+        <v>29152847</v>
+      </c>
+      <c r="B199">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2">
+      <c r="A200">
+        <v>29531332</v>
+      </c>
+      <c r="B200">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2">
+      <c r="A201">
+        <v>30697379</v>
+      </c>
+      <c r="B201">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A101">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="324717928">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="324717928">
       <formula>NOT(ISERROR(SEARCH("324717928",A2)))</formula>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A101">
+    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A201">
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A102:A201">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
carga ingreso, personal y personalxingreso
</commit_message>
<xml_diff>
--- a/Excel/Carga DB Postgres/PersonalXIngreso - cargado.xlsx
+++ b/Excel/Carga DB Postgres/PersonalXIngreso - cargado.xlsx
@@ -1664,7 +1664,7 @@
   <dimension ref="A1:B201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102:A201"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1683,7 +1683,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>32096467</v>
+        <v>19262658</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1691,7 +1691,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>20647870</v>
+        <v>25863441</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1699,7 +1699,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>20347118</v>
+        <v>23397823</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -1707,7 +1707,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>25574544</v>
+        <v>15521344</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1715,7 +1715,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>29585676</v>
+        <v>20842822</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -1723,7 +1723,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>26868305</v>
+        <v>21479306</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -1731,7 +1731,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>19980772</v>
+        <v>15655702</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -1739,7 +1739,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>24686460</v>
+        <v>16076433</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -1747,7 +1747,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>22554028</v>
+        <v>29629311</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -1755,7 +1755,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>19245391</v>
+        <v>17796646</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -1763,7 +1763,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>18041182</v>
+        <v>33753109</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -1771,7 +1771,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>25167480</v>
+        <v>18960031</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -1779,7 +1779,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
-        <v>21285840</v>
+        <v>27348400</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -1787,7 +1787,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
-        <v>27520532</v>
+        <v>24626175</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -1795,7 +1795,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16">
-        <v>24572930</v>
+        <v>20183587</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -1803,7 +1803,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17">
-        <v>34557321</v>
+        <v>21493242</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -1811,7 +1811,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18">
-        <v>29795794</v>
+        <v>33388216</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -1819,7 +1819,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19">
-        <v>21640394</v>
+        <v>29705002</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -1827,7 +1827,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20">
-        <v>31657842</v>
+        <v>17509586</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -1835,7 +1835,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21">
-        <v>18944096</v>
+        <v>33454923</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -1843,7 +1843,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22">
-        <v>31965824</v>
+        <v>33910408</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -1851,7 +1851,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23">
-        <v>17592277</v>
+        <v>25056740</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -1859,7 +1859,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24">
-        <v>21814714</v>
+        <v>15145164</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -1867,7 +1867,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25">
-        <v>18131354</v>
+        <v>32303477</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -1875,7 +1875,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26">
-        <v>24316104</v>
+        <v>25201796</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -1883,7 +1883,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27">
-        <v>34974848</v>
+        <v>16676378</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -1891,7 +1891,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28">
-        <v>18837447</v>
+        <v>15775013</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -1899,7 +1899,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29">
-        <v>27047705</v>
+        <v>20794916</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -1907,7 +1907,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30">
-        <v>24589925</v>
+        <v>32861591</v>
       </c>
       <c r="B30">
         <v>29</v>
@@ -1915,7 +1915,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31">
-        <v>26845383</v>
+        <v>32916260</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -1923,7 +1923,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32">
-        <v>27703543</v>
+        <v>16198380</v>
       </c>
       <c r="B32">
         <v>31</v>
@@ -1931,7 +1931,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33">
-        <v>25489762</v>
+        <v>31583118</v>
       </c>
       <c r="B33">
         <v>32</v>
@@ -1939,7 +1939,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34">
-        <v>19036988</v>
+        <v>29830955</v>
       </c>
       <c r="B34">
         <v>33</v>
@@ -1947,7 +1947,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35">
-        <v>15755794</v>
+        <v>28807477</v>
       </c>
       <c r="B35">
         <v>34</v>
@@ -1955,7 +1955,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36">
-        <v>20897843</v>
+        <v>15499357</v>
       </c>
       <c r="B36">
         <v>35</v>
@@ -1963,7 +1963,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37">
-        <v>34239679</v>
+        <v>34416555</v>
       </c>
       <c r="B37">
         <v>36</v>
@@ -1971,7 +1971,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38">
-        <v>26551089</v>
+        <v>17675854</v>
       </c>
       <c r="B38">
         <v>37</v>
@@ -1979,7 +1979,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39">
-        <v>18557593</v>
+        <v>19531368</v>
       </c>
       <c r="B39">
         <v>38</v>
@@ -1987,7 +1987,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40">
-        <v>25098867</v>
+        <v>22214183</v>
       </c>
       <c r="B40">
         <v>39</v>
@@ -1995,7 +1995,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41">
-        <v>27604761</v>
+        <v>20397678</v>
       </c>
       <c r="B41">
         <v>40</v>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42">
-        <v>25581528</v>
+        <v>22512767</v>
       </c>
       <c r="B42">
         <v>41</v>
@@ -2011,7 +2011,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43">
-        <v>32837992</v>
+        <v>23789137</v>
       </c>
       <c r="B43">
         <v>42</v>
@@ -2019,7 +2019,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44">
-        <v>29042728</v>
+        <v>24740276</v>
       </c>
       <c r="B44">
         <v>43</v>
@@ -2027,7 +2027,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45">
-        <v>23389737</v>
+        <v>15374593</v>
       </c>
       <c r="B45">
         <v>44</v>
@@ -2035,7 +2035,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46">
-        <v>23187345</v>
+        <v>32945116</v>
       </c>
       <c r="B46">
         <v>45</v>
@@ -2043,7 +2043,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47">
-        <v>27942195</v>
+        <v>20876602</v>
       </c>
       <c r="B47">
         <v>46</v>
@@ -2051,7 +2051,7 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48">
-        <v>31152632</v>
+        <v>26126426</v>
       </c>
       <c r="B48">
         <v>47</v>
@@ -2059,7 +2059,7 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49">
-        <v>15969214</v>
+        <v>23811015</v>
       </c>
       <c r="B49">
         <v>48</v>
@@ -2067,7 +2067,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50">
-        <v>30976043</v>
+        <v>33559776</v>
       </c>
       <c r="B50">
         <v>49</v>
@@ -2075,7 +2075,7 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51">
-        <v>24672474</v>
+        <v>20665949</v>
       </c>
       <c r="B51">
         <v>50</v>
@@ -2083,7 +2083,7 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52">
-        <v>24642604</v>
+        <v>25781940</v>
       </c>
       <c r="B52">
         <v>51</v>
@@ -2091,7 +2091,7 @@
     </row>
     <row r="53" spans="1:2">
       <c r="A53">
-        <v>31642295</v>
+        <v>30483998</v>
       </c>
       <c r="B53">
         <v>52</v>
@@ -2099,7 +2099,7 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54">
-        <v>27529809</v>
+        <v>19954328</v>
       </c>
       <c r="B54">
         <v>53</v>
@@ -2107,7 +2107,7 @@
     </row>
     <row r="55" spans="1:2">
       <c r="A55">
-        <v>24262103</v>
+        <v>23352064</v>
       </c>
       <c r="B55">
         <v>54</v>
@@ -2115,7 +2115,7 @@
     </row>
     <row r="56" spans="1:2">
       <c r="A56">
-        <v>22207525</v>
+        <v>32303270</v>
       </c>
       <c r="B56">
         <v>55</v>
@@ -2123,7 +2123,7 @@
     </row>
     <row r="57" spans="1:2">
       <c r="A57">
-        <v>16187044</v>
+        <v>20567193</v>
       </c>
       <c r="B57">
         <v>56</v>
@@ -2131,7 +2131,7 @@
     </row>
     <row r="58" spans="1:2">
       <c r="A58">
-        <v>25153656</v>
+        <v>31518105</v>
       </c>
       <c r="B58">
         <v>57</v>
@@ -2139,7 +2139,7 @@
     </row>
     <row r="59" spans="1:2">
       <c r="A59">
-        <v>17985423</v>
+        <v>15421676</v>
       </c>
       <c r="B59">
         <v>58</v>
@@ -2147,7 +2147,7 @@
     </row>
     <row r="60" spans="1:2">
       <c r="A60">
-        <v>30641872</v>
+        <v>24172605</v>
       </c>
       <c r="B60">
         <v>59</v>
@@ -2155,7 +2155,7 @@
     </row>
     <row r="61" spans="1:2">
       <c r="A61">
-        <v>18839338</v>
+        <v>28119037</v>
       </c>
       <c r="B61">
         <v>60</v>
@@ -2163,7 +2163,7 @@
     </row>
     <row r="62" spans="1:2">
       <c r="A62">
-        <v>31473787</v>
+        <v>27727477</v>
       </c>
       <c r="B62">
         <v>61</v>
@@ -2171,7 +2171,7 @@
     </row>
     <row r="63" spans="1:2">
       <c r="A63">
-        <v>28558962</v>
+        <v>29697651</v>
       </c>
       <c r="B63">
         <v>62</v>
@@ -2179,7 +2179,7 @@
     </row>
     <row r="64" spans="1:2">
       <c r="A64">
-        <v>17923094</v>
+        <v>17643972</v>
       </c>
       <c r="B64">
         <v>63</v>
@@ -2187,7 +2187,7 @@
     </row>
     <row r="65" spans="1:2">
       <c r="A65">
-        <v>34358608</v>
+        <v>26337848</v>
       </c>
       <c r="B65">
         <v>64</v>
@@ -2195,7 +2195,7 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66">
-        <v>21878506</v>
+        <v>25256060</v>
       </c>
       <c r="B66">
         <v>65</v>
@@ -2203,7 +2203,7 @@
     </row>
     <row r="67" spans="1:2">
       <c r="A67">
-        <v>17048816</v>
+        <v>17188039</v>
       </c>
       <c r="B67">
         <v>66</v>
@@ -2211,7 +2211,7 @@
     </row>
     <row r="68" spans="1:2">
       <c r="A68">
-        <v>32253538</v>
+        <v>25814706</v>
       </c>
       <c r="B68">
         <v>67</v>
@@ -2219,7 +2219,7 @@
     </row>
     <row r="69" spans="1:2">
       <c r="A69">
-        <v>25203547</v>
+        <v>26991038</v>
       </c>
       <c r="B69">
         <v>68</v>
@@ -2227,7 +2227,7 @@
     </row>
     <row r="70" spans="1:2">
       <c r="A70">
-        <v>33028506</v>
+        <v>34586368</v>
       </c>
       <c r="B70">
         <v>69</v>
@@ -2235,7 +2235,7 @@
     </row>
     <row r="71" spans="1:2">
       <c r="A71">
-        <v>31656189</v>
+        <v>24289844</v>
       </c>
       <c r="B71">
         <v>70</v>
@@ -2243,7 +2243,7 @@
     </row>
     <row r="72" spans="1:2">
       <c r="A72">
-        <v>24463672</v>
+        <v>17342085</v>
       </c>
       <c r="B72">
         <v>71</v>
@@ -2251,7 +2251,7 @@
     </row>
     <row r="73" spans="1:2">
       <c r="A73">
-        <v>16940172</v>
+        <v>15969084</v>
       </c>
       <c r="B73">
         <v>72</v>
@@ -2259,7 +2259,7 @@
     </row>
     <row r="74" spans="1:2">
       <c r="A74">
-        <v>24149517</v>
+        <v>30637498</v>
       </c>
       <c r="B74">
         <v>73</v>
@@ -2267,7 +2267,7 @@
     </row>
     <row r="75" spans="1:2">
       <c r="A75">
-        <v>18920859</v>
+        <v>22927639</v>
       </c>
       <c r="B75">
         <v>74</v>
@@ -2275,7 +2275,7 @@
     </row>
     <row r="76" spans="1:2">
       <c r="A76">
-        <v>27569447</v>
+        <v>19119097</v>
       </c>
       <c r="B76">
         <v>75</v>
@@ -2283,7 +2283,7 @@
     </row>
     <row r="77" spans="1:2">
       <c r="A77">
-        <v>30925256</v>
+        <v>27551675</v>
       </c>
       <c r="B77">
         <v>76</v>
@@ -2291,7 +2291,7 @@
     </row>
     <row r="78" spans="1:2">
       <c r="A78">
-        <v>30054231</v>
+        <v>20917644</v>
       </c>
       <c r="B78">
         <v>77</v>
@@ -2299,7 +2299,7 @@
     </row>
     <row r="79" spans="1:2">
       <c r="A79">
-        <v>22166629</v>
+        <v>24307549</v>
       </c>
       <c r="B79">
         <v>78</v>
@@ -2307,7 +2307,7 @@
     </row>
     <row r="80" spans="1:2">
       <c r="A80">
-        <v>19119398</v>
+        <v>30467368</v>
       </c>
       <c r="B80">
         <v>79</v>
@@ -2315,7 +2315,7 @@
     </row>
     <row r="81" spans="1:2">
       <c r="A81">
-        <v>22673405</v>
+        <v>32237069</v>
       </c>
       <c r="B81">
         <v>80</v>
@@ -2323,7 +2323,7 @@
     </row>
     <row r="82" spans="1:2">
       <c r="A82">
-        <v>28415922</v>
+        <v>34053665</v>
       </c>
       <c r="B82">
         <v>81</v>
@@ -2331,7 +2331,7 @@
     </row>
     <row r="83" spans="1:2">
       <c r="A83">
-        <v>23622405</v>
+        <v>18123265</v>
       </c>
       <c r="B83">
         <v>82</v>
@@ -2339,7 +2339,7 @@
     </row>
     <row r="84" spans="1:2">
       <c r="A84">
-        <v>33072109</v>
+        <v>19008640</v>
       </c>
       <c r="B84">
         <v>83</v>
@@ -2347,7 +2347,7 @@
     </row>
     <row r="85" spans="1:2">
       <c r="A85">
-        <v>23421776</v>
+        <v>20321880</v>
       </c>
       <c r="B85">
         <v>84</v>
@@ -2355,7 +2355,7 @@
     </row>
     <row r="86" spans="1:2">
       <c r="A86">
-        <v>26071335</v>
+        <v>16785183</v>
       </c>
       <c r="B86">
         <v>85</v>
@@ -2363,7 +2363,7 @@
     </row>
     <row r="87" spans="1:2">
       <c r="A87">
-        <v>24263836</v>
+        <v>15924934</v>
       </c>
       <c r="B87">
         <v>86</v>
@@ -2371,7 +2371,7 @@
     </row>
     <row r="88" spans="1:2">
       <c r="A88">
-        <v>19339218</v>
+        <v>33161037</v>
       </c>
       <c r="B88">
         <v>87</v>
@@ -2379,7 +2379,7 @@
     </row>
     <row r="89" spans="1:2">
       <c r="A89">
-        <v>34837359</v>
+        <v>26732978</v>
       </c>
       <c r="B89">
         <v>88</v>
@@ -2387,7 +2387,7 @@
     </row>
     <row r="90" spans="1:2">
       <c r="A90">
-        <v>18968297</v>
+        <v>18256192</v>
       </c>
       <c r="B90">
         <v>89</v>
@@ -2395,7 +2395,7 @@
     </row>
     <row r="91" spans="1:2">
       <c r="A91">
-        <v>25381386</v>
+        <v>34760631</v>
       </c>
       <c r="B91">
         <v>90</v>
@@ -2403,7 +2403,7 @@
     </row>
     <row r="92" spans="1:2">
       <c r="A92">
-        <v>32492863</v>
+        <v>27871571</v>
       </c>
       <c r="B92">
         <v>91</v>
@@ -2411,7 +2411,7 @@
     </row>
     <row r="93" spans="1:2">
       <c r="A93">
-        <v>29050116</v>
+        <v>31830055</v>
       </c>
       <c r="B93">
         <v>92</v>
@@ -2419,7 +2419,7 @@
     </row>
     <row r="94" spans="1:2">
       <c r="A94">
-        <v>32465702</v>
+        <v>26177582</v>
       </c>
       <c r="B94">
         <v>93</v>
@@ -2427,7 +2427,7 @@
     </row>
     <row r="95" spans="1:2">
       <c r="A95">
-        <v>30487701</v>
+        <v>34174468</v>
       </c>
       <c r="B95">
         <v>94</v>
@@ -2435,7 +2435,7 @@
     </row>
     <row r="96" spans="1:2">
       <c r="A96">
-        <v>33601679</v>
+        <v>15412176</v>
       </c>
       <c r="B96">
         <v>95</v>
@@ -2443,7 +2443,7 @@
     </row>
     <row r="97" spans="1:2">
       <c r="A97">
-        <v>29810406</v>
+        <v>34723160</v>
       </c>
       <c r="B97">
         <v>96</v>
@@ -2451,7 +2451,7 @@
     </row>
     <row r="98" spans="1:2">
       <c r="A98">
-        <v>15051339</v>
+        <v>19332742</v>
       </c>
       <c r="B98">
         <v>97</v>
@@ -2459,7 +2459,7 @@
     </row>
     <row r="99" spans="1:2">
       <c r="A99">
-        <v>17133023</v>
+        <v>33479482</v>
       </c>
       <c r="B99">
         <v>98</v>
@@ -2467,7 +2467,7 @@
     </row>
     <row r="100" spans="1:2">
       <c r="A100">
-        <v>20559239</v>
+        <v>30802527</v>
       </c>
       <c r="B100">
         <v>99</v>
@@ -2475,828 +2475,532 @@
     </row>
     <row r="101" spans="1:2">
       <c r="A101">
-        <v>28910722</v>
+        <v>30924687</v>
       </c>
       <c r="B101">
         <v>100</v>
       </c>
     </row>
     <row r="102" spans="1:2">
-      <c r="A102">
-        <v>26091292</v>
-      </c>
       <c r="B102">
         <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:2">
-      <c r="A103">
-        <v>22812890</v>
-      </c>
       <c r="B103">
         <v>2</v>
       </c>
     </row>
     <row r="104" spans="1:2">
-      <c r="A104">
-        <v>27535553</v>
-      </c>
       <c r="B104">
         <v>3</v>
       </c>
     </row>
     <row r="105" spans="1:2">
-      <c r="A105">
-        <v>30914580</v>
-      </c>
       <c r="B105">
         <v>4</v>
       </c>
     </row>
     <row r="106" spans="1:2">
-      <c r="A106">
-        <v>24717521</v>
-      </c>
       <c r="B106">
         <v>5</v>
       </c>
     </row>
     <row r="107" spans="1:2">
-      <c r="A107">
-        <v>23628653</v>
-      </c>
       <c r="B107">
         <v>6</v>
       </c>
     </row>
     <row r="108" spans="1:2">
-      <c r="A108">
-        <v>30448578</v>
-      </c>
       <c r="B108">
         <v>7</v>
       </c>
     </row>
     <row r="109" spans="1:2">
-      <c r="A109">
-        <v>28196547</v>
-      </c>
       <c r="B109">
         <v>8</v>
       </c>
     </row>
     <row r="110" spans="1:2">
-      <c r="A110">
-        <v>16492021</v>
-      </c>
       <c r="B110">
         <v>9</v>
       </c>
     </row>
     <row r="111" spans="1:2">
-      <c r="A111">
-        <v>35380958</v>
-      </c>
       <c r="B111">
         <v>10</v>
       </c>
     </row>
     <row r="112" spans="1:2">
-      <c r="A112">
-        <v>22351087</v>
-      </c>
       <c r="B112">
         <v>11</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
-      <c r="A113">
-        <v>27061739</v>
-      </c>
+    <row r="113" spans="2:2">
       <c r="B113">
         <v>12</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
-      <c r="A114">
-        <v>23876879</v>
-      </c>
+    <row r="114" spans="2:2">
       <c r="B114">
         <v>13</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
-      <c r="A115">
-        <v>32111599</v>
-      </c>
+    <row r="115" spans="2:2">
       <c r="B115">
         <v>14</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
-      <c r="A116">
-        <v>30407599</v>
-      </c>
+    <row r="116" spans="2:2">
       <c r="B116">
         <v>15</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
-      <c r="A117">
-        <v>25231611</v>
-      </c>
+    <row r="117" spans="2:2">
       <c r="B117">
         <v>16</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
-      <c r="A118">
-        <v>23672861</v>
-      </c>
+    <row r="118" spans="2:2">
       <c r="B118">
         <v>17</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
-      <c r="A119">
-        <v>26756360</v>
-      </c>
+    <row r="119" spans="2:2">
       <c r="B119">
         <v>18</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
-      <c r="A120">
-        <v>24756508</v>
-      </c>
+    <row r="120" spans="2:2">
       <c r="B120">
         <v>19</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
-      <c r="A121">
-        <v>18545884</v>
-      </c>
+    <row r="121" spans="2:2">
       <c r="B121">
         <v>20</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
-      <c r="A122">
-        <v>24405970</v>
-      </c>
+    <row r="122" spans="2:2">
       <c r="B122">
         <v>21</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
-      <c r="A123">
-        <v>25370464</v>
-      </c>
+    <row r="123" spans="2:2">
       <c r="B123">
         <v>22</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
-      <c r="A124">
-        <v>32439727</v>
-      </c>
+    <row r="124" spans="2:2">
       <c r="B124">
         <v>23</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
-      <c r="A125">
-        <v>31937562</v>
-      </c>
+    <row r="125" spans="2:2">
       <c r="B125">
         <v>24</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
-      <c r="A126">
-        <v>30276531</v>
-      </c>
+    <row r="126" spans="2:2">
       <c r="B126">
         <v>25</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
-      <c r="A127">
-        <v>13348995</v>
-      </c>
+    <row r="127" spans="2:2">
       <c r="B127">
         <v>26</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
-      <c r="A128">
-        <v>35957660</v>
-      </c>
+    <row r="128" spans="2:2">
       <c r="B128">
         <v>27</v>
       </c>
     </row>
-    <row r="129" spans="1:2">
-      <c r="A129">
-        <v>10000278</v>
-      </c>
+    <row r="129" spans="2:2">
       <c r="B129">
         <v>28</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
-      <c r="A130">
-        <v>26169317</v>
-      </c>
+    <row r="130" spans="2:2">
       <c r="B130">
         <v>29</v>
       </c>
     </row>
-    <row r="131" spans="1:2">
-      <c r="A131">
-        <v>23413527</v>
-      </c>
+    <row r="131" spans="2:2">
       <c r="B131">
         <v>30</v>
       </c>
     </row>
-    <row r="132" spans="1:2">
-      <c r="A132">
-        <v>26043475</v>
-      </c>
+    <row r="132" spans="2:2">
       <c r="B132">
         <v>31</v>
       </c>
     </row>
-    <row r="133" spans="1:2">
-      <c r="A133">
-        <v>31292018</v>
-      </c>
+    <row r="133" spans="2:2">
       <c r="B133">
         <v>32</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
-      <c r="A134">
-        <v>24922379</v>
-      </c>
+    <row r="134" spans="2:2">
       <c r="B134">
         <v>33</v>
       </c>
     </row>
-    <row r="135" spans="1:2">
-      <c r="A135">
-        <v>22288009</v>
-      </c>
+    <row r="135" spans="2:2">
       <c r="B135">
         <v>34</v>
       </c>
     </row>
-    <row r="136" spans="1:2">
-      <c r="A136">
-        <v>22574668</v>
-      </c>
+    <row r="136" spans="2:2">
       <c r="B136">
         <v>35</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
-      <c r="A137">
-        <v>27284020</v>
-      </c>
+    <row r="137" spans="2:2">
       <c r="B137">
         <v>36</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
-      <c r="A138">
-        <v>93791921</v>
-      </c>
+    <row r="138" spans="2:2">
       <c r="B138">
         <v>37</v>
       </c>
     </row>
-    <row r="139" spans="1:2">
-      <c r="A139">
-        <v>24336922</v>
-      </c>
+    <row r="139" spans="2:2">
       <c r="B139">
         <v>38</v>
       </c>
     </row>
-    <row r="140" spans="1:2">
-      <c r="A140">
-        <v>32638727</v>
-      </c>
+    <row r="140" spans="2:2">
       <c r="B140">
         <v>39</v>
       </c>
     </row>
-    <row r="141" spans="1:2">
-      <c r="A141">
-        <v>36403885</v>
-      </c>
+    <row r="141" spans="2:2">
       <c r="B141">
         <v>40</v>
       </c>
     </row>
-    <row r="142" spans="1:2">
-      <c r="A142">
-        <v>31477190</v>
-      </c>
+    <row r="142" spans="2:2">
       <c r="B142">
         <v>41</v>
       </c>
     </row>
-    <row r="143" spans="1:2">
-      <c r="A143">
-        <v>25182981</v>
-      </c>
+    <row r="143" spans="2:2">
       <c r="B143">
         <v>42</v>
       </c>
     </row>
-    <row r="144" spans="1:2">
-      <c r="A144">
-        <v>26965196</v>
-      </c>
+    <row r="144" spans="2:2">
       <c r="B144">
         <v>43</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
-      <c r="A145">
-        <v>32091714</v>
-      </c>
+    <row r="145" spans="2:2">
       <c r="B145">
         <v>44</v>
       </c>
     </row>
-    <row r="146" spans="1:2">
-      <c r="A146">
-        <v>30815197</v>
-      </c>
+    <row r="146" spans="2:2">
       <c r="B146">
         <v>45</v>
       </c>
     </row>
-    <row r="147" spans="1:2">
-      <c r="A147">
-        <v>22666665</v>
-      </c>
+    <row r="147" spans="2:2">
       <c r="B147">
         <v>46</v>
       </c>
     </row>
-    <row r="148" spans="1:2">
-      <c r="A148">
-        <v>29867735</v>
-      </c>
+    <row r="148" spans="2:2">
       <c r="B148">
         <v>47</v>
       </c>
     </row>
-    <row r="149" spans="1:2">
-      <c r="A149">
-        <v>31752457</v>
-      </c>
+    <row r="149" spans="2:2">
       <c r="B149">
         <v>48</v>
       </c>
     </row>
-    <row r="150" spans="1:2">
-      <c r="A150">
-        <v>29702373</v>
-      </c>
+    <row r="150" spans="2:2">
       <c r="B150">
         <v>49</v>
       </c>
     </row>
-    <row r="151" spans="1:2">
-      <c r="A151">
-        <v>25847587</v>
-      </c>
+    <row r="151" spans="2:2">
       <c r="B151">
         <v>50</v>
       </c>
     </row>
-    <row r="152" spans="1:2">
-      <c r="A152">
-        <v>20520064</v>
-      </c>
+    <row r="152" spans="2:2">
       <c r="B152">
         <v>51</v>
       </c>
     </row>
-    <row r="153" spans="1:2">
-      <c r="A153">
-        <v>33017487</v>
-      </c>
+    <row r="153" spans="2:2">
       <c r="B153">
         <v>52</v>
       </c>
     </row>
-    <row r="154" spans="1:2">
-      <c r="A154">
-        <v>21818154</v>
-      </c>
+    <row r="154" spans="2:2">
       <c r="B154">
         <v>53</v>
       </c>
     </row>
-    <row r="155" spans="1:2">
-      <c r="A155">
-        <v>36921072</v>
-      </c>
+    <row r="155" spans="2:2">
       <c r="B155">
         <v>54</v>
       </c>
     </row>
-    <row r="156" spans="1:2">
-      <c r="A156">
-        <v>22195367</v>
-      </c>
+    <row r="156" spans="2:2">
       <c r="B156">
         <v>55</v>
       </c>
     </row>
-    <row r="157" spans="1:2">
-      <c r="A157">
-        <v>21972573</v>
-      </c>
+    <row r="157" spans="2:2">
       <c r="B157">
         <v>56</v>
       </c>
     </row>
-    <row r="158" spans="1:2">
-      <c r="A158">
-        <v>26127463</v>
-      </c>
+    <row r="158" spans="2:2">
       <c r="B158">
         <v>57</v>
       </c>
     </row>
-    <row r="159" spans="1:2">
-      <c r="A159">
-        <v>30934859</v>
-      </c>
+    <row r="159" spans="2:2">
       <c r="B159">
         <v>58</v>
       </c>
     </row>
-    <row r="160" spans="1:2">
-      <c r="A160">
-        <v>26328066</v>
-      </c>
+    <row r="160" spans="2:2">
       <c r="B160">
         <v>59</v>
       </c>
     </row>
-    <row r="161" spans="1:2">
-      <c r="A161">
-        <v>33391190</v>
-      </c>
+    <row r="161" spans="2:2">
       <c r="B161">
         <v>60</v>
       </c>
     </row>
-    <row r="162" spans="1:2">
-      <c r="A162">
-        <v>27486398</v>
-      </c>
+    <row r="162" spans="2:2">
       <c r="B162">
         <v>61</v>
       </c>
     </row>
-    <row r="163" spans="1:2">
-      <c r="A163">
-        <v>30410289</v>
-      </c>
+    <row r="163" spans="2:2">
       <c r="B163">
         <v>62</v>
       </c>
     </row>
-    <row r="164" spans="1:2">
-      <c r="A164">
-        <v>27146494</v>
-      </c>
+    <row r="164" spans="2:2">
       <c r="B164">
         <v>63</v>
       </c>
     </row>
-    <row r="165" spans="1:2">
-      <c r="A165">
-        <v>26387145</v>
-      </c>
+    <row r="165" spans="2:2">
       <c r="B165">
         <v>64</v>
       </c>
     </row>
-    <row r="166" spans="1:2">
-      <c r="A166">
-        <v>26604529</v>
-      </c>
+    <row r="166" spans="2:2">
       <c r="B166">
         <v>65</v>
       </c>
     </row>
-    <row r="167" spans="1:2">
-      <c r="A167">
-        <v>31963375</v>
-      </c>
+    <row r="167" spans="2:2">
       <c r="B167">
         <v>66</v>
       </c>
     </row>
-    <row r="168" spans="1:2">
-      <c r="A168">
-        <v>27383550</v>
-      </c>
+    <row r="168" spans="2:2">
       <c r="B168">
         <v>67</v>
       </c>
     </row>
-    <row r="169" spans="1:2">
-      <c r="A169">
-        <v>18808701</v>
-      </c>
+    <row r="169" spans="2:2">
       <c r="B169">
         <v>68</v>
       </c>
     </row>
-    <row r="170" spans="1:2">
-      <c r="A170">
-        <v>25529423</v>
-      </c>
+    <row r="170" spans="2:2">
       <c r="B170">
         <v>69</v>
       </c>
     </row>
-    <row r="171" spans="1:2">
-      <c r="A171">
-        <v>39664632</v>
-      </c>
+    <row r="171" spans="2:2">
       <c r="B171">
         <v>70</v>
       </c>
     </row>
-    <row r="172" spans="1:2">
-      <c r="A172">
-        <v>25822174</v>
-      </c>
+    <row r="172" spans="2:2">
       <c r="B172">
         <v>71</v>
       </c>
     </row>
-    <row r="173" spans="1:2">
-      <c r="A173">
-        <v>30218532</v>
-      </c>
+    <row r="173" spans="2:2">
       <c r="B173">
         <v>72</v>
       </c>
     </row>
-    <row r="174" spans="1:2">
-      <c r="A174">
-        <v>29158026</v>
-      </c>
+    <row r="174" spans="2:2">
       <c r="B174">
         <v>73</v>
       </c>
     </row>
-    <row r="175" spans="1:2">
-      <c r="A175">
-        <v>35122148</v>
-      </c>
+    <row r="175" spans="2:2">
       <c r="B175">
         <v>74</v>
       </c>
     </row>
-    <row r="176" spans="1:2">
-      <c r="A176">
-        <v>32983368</v>
-      </c>
+    <row r="176" spans="2:2">
       <c r="B176">
         <v>75</v>
       </c>
     </row>
-    <row r="177" spans="1:2">
-      <c r="A177">
-        <v>23050239</v>
-      </c>
+    <row r="177" spans="2:2">
       <c r="B177">
         <v>76</v>
       </c>
     </row>
-    <row r="178" spans="1:2">
-      <c r="A178">
-        <v>94217792</v>
-      </c>
+    <row r="178" spans="2:2">
       <c r="B178">
         <v>77</v>
       </c>
     </row>
-    <row r="179" spans="1:2">
-      <c r="A179">
-        <v>31929128</v>
-      </c>
+    <row r="179" spans="2:2">
       <c r="B179">
         <v>78</v>
       </c>
     </row>
-    <row r="180" spans="1:2">
-      <c r="A180">
-        <v>18631066</v>
-      </c>
+    <row r="180" spans="2:2">
       <c r="B180">
         <v>79</v>
       </c>
     </row>
-    <row r="181" spans="1:2">
-      <c r="A181">
-        <v>17726061</v>
-      </c>
+    <row r="181" spans="2:2">
       <c r="B181">
         <v>80</v>
       </c>
     </row>
-    <row r="182" spans="1:2">
-      <c r="A182">
-        <v>25988906</v>
-      </c>
+    <row r="182" spans="2:2">
       <c r="B182">
         <v>81</v>
       </c>
     </row>
-    <row r="183" spans="1:2">
-      <c r="A183">
-        <v>34519429</v>
-      </c>
+    <row r="183" spans="2:2">
       <c r="B183">
         <v>82</v>
       </c>
     </row>
-    <row r="184" spans="1:2">
-      <c r="A184">
-        <v>25675517</v>
-      </c>
+    <row r="184" spans="2:2">
       <c r="B184">
         <v>83</v>
       </c>
     </row>
-    <row r="185" spans="1:2">
-      <c r="A185">
-        <v>30586320</v>
-      </c>
+    <row r="185" spans="2:2">
       <c r="B185">
         <v>84</v>
       </c>
     </row>
-    <row r="186" spans="1:2">
-      <c r="A186">
-        <v>29250659</v>
-      </c>
+    <row r="186" spans="2:2">
       <c r="B186">
         <v>85</v>
       </c>
     </row>
-    <row r="187" spans="1:2">
-      <c r="A187">
-        <v>24905953</v>
-      </c>
+    <row r="187" spans="2:2">
       <c r="B187">
         <v>86</v>
       </c>
     </row>
-    <row r="188" spans="1:2">
-      <c r="A188">
-        <v>31342470</v>
-      </c>
+    <row r="188" spans="2:2">
       <c r="B188">
         <v>87</v>
       </c>
     </row>
-    <row r="189" spans="1:2">
-      <c r="A189">
-        <v>27152292</v>
-      </c>
+    <row r="189" spans="2:2">
       <c r="B189">
         <v>88</v>
       </c>
     </row>
-    <row r="190" spans="1:2">
-      <c r="A190">
-        <v>33780102</v>
-      </c>
+    <row r="190" spans="2:2">
       <c r="B190">
         <v>89</v>
       </c>
     </row>
-    <row r="191" spans="1:2">
-      <c r="A191">
-        <v>29799190</v>
-      </c>
+    <row r="191" spans="2:2">
       <c r="B191">
         <v>90</v>
       </c>
     </row>
-    <row r="192" spans="1:2">
-      <c r="A192">
-        <v>36461022</v>
-      </c>
+    <row r="192" spans="2:2">
       <c r="B192">
         <v>91</v>
       </c>
     </row>
-    <row r="193" spans="1:2">
-      <c r="A193">
-        <v>12683815</v>
-      </c>
+    <row r="193" spans="2:2">
       <c r="B193">
         <v>92</v>
       </c>
     </row>
-    <row r="194" spans="1:2">
-      <c r="A194">
-        <v>36594138</v>
-      </c>
+    <row r="194" spans="2:2">
       <c r="B194">
         <v>93</v>
       </c>
     </row>
-    <row r="195" spans="1:2">
-      <c r="A195">
-        <v>29906783</v>
-      </c>
+    <row r="195" spans="2:2">
       <c r="B195">
         <v>94</v>
       </c>
     </row>
-    <row r="196" spans="1:2">
-      <c r="A196">
-        <v>36684361</v>
-      </c>
+    <row r="196" spans="2:2">
       <c r="B196">
         <v>95</v>
       </c>
     </row>
-    <row r="197" spans="1:2">
-      <c r="A197">
-        <v>28825557</v>
-      </c>
+    <row r="197" spans="2:2">
       <c r="B197">
         <v>96</v>
       </c>
     </row>
-    <row r="198" spans="1:2">
-      <c r="A198">
-        <v>35141683</v>
-      </c>
+    <row r="198" spans="2:2">
       <c r="B198">
         <v>97</v>
       </c>
     </row>
-    <row r="199" spans="1:2">
-      <c r="A199">
-        <v>29152847</v>
-      </c>
+    <row r="199" spans="2:2">
       <c r="B199">
         <v>98</v>
       </c>
     </row>
-    <row r="200" spans="1:2">
-      <c r="A200">
-        <v>29531332</v>
-      </c>
+    <row r="200" spans="2:2">
       <c r="B200">
         <v>99</v>
       </c>
     </row>
-    <row r="201" spans="1:2">
-      <c r="A201">
-        <v>30697379</v>
-      </c>
+    <row r="201" spans="2:2">
       <c r="B201">
         <v>100</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A101">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="324717928">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="324717928">
       <formula>NOT(ISERROR(SEARCH("324717928",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A101">
-    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A201">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A102:A201">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A101">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>